<commit_message>
Classifying Files through options
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBIT\Second Semester\EE\Project\Engineering-Exploration-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96187656-898D-4312-A8A6-F40337E66727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18976329-1818-405F-BAC6-155FF92F5774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Sno</t>
   </si>
@@ -39,7 +39,88 @@
     <t>Email id</t>
   </si>
   <si>
-    <t>Marks</t>
+    <t>Choices</t>
+  </si>
+  <si>
+    <t>ASDF</t>
+  </si>
+  <si>
+    <t>qdy dfef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qrtyw </t>
+  </si>
+  <si>
+    <t>aassw</t>
+  </si>
+  <si>
+    <t>weff_</t>
+  </si>
+  <si>
+    <t>eef</t>
+  </si>
+  <si>
+    <t>deed</t>
+  </si>
+  <si>
+    <t>dffc</t>
+  </si>
+  <si>
+    <t>eefv</t>
+  </si>
+  <si>
+    <t>efccc</t>
+  </si>
+  <si>
+    <t>qwertyuio</t>
+  </si>
+  <si>
+    <t>asdfghjkl</t>
+  </si>
+  <si>
+    <t>sdfghjkl;</t>
+  </si>
+  <si>
+    <t>dfghjkl</t>
+  </si>
+  <si>
+    <t>poiuytgfrd</t>
+  </si>
+  <si>
+    <t>xcvbnm,</t>
+  </si>
+  <si>
+    <t>xcvbnm,.</t>
+  </si>
+  <si>
+    <t>plkjnhgfd</t>
+  </si>
+  <si>
+    <t>A,B,C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A,B,C,D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A,B,C,D,E</t>
+  </si>
+  <si>
+    <t>B, C</t>
   </si>
 </sst>
 </file>
@@ -357,13 +438,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -382,6 +467,176 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Form Sorting, except titles completed. Added icons
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBIT\Second Semester\EE\Project\Engineering-Exploration-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C6F8AF-4A36-4496-AA4A-A92980A787AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7831FE-ADF7-4361-B90D-BD9C6E4B3AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Sno</t>
   </si>
@@ -66,9 +66,6 @@
     <t>deed</t>
   </si>
   <si>
-    <t>dffc</t>
-  </si>
-  <si>
     <t>eefv</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
   </si>
   <si>
     <t>A, B, C, D</t>
-  </si>
-  <si>
-    <t>A,B, C,D    ,    E</t>
   </si>
   <si>
     <t>B,  C</t>
@@ -444,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -488,10 +482,10 @@
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>74123698</v>
@@ -508,10 +502,10 @@
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>852698</v>
@@ -528,10 +522,10 @@
         <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>741</v>
@@ -548,10 +542,10 @@
         <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>123698</v>
@@ -568,10 +562,10 @@
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6">
         <v>962147</v>
@@ -588,10 +582,10 @@
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7">
         <v>412</v>
@@ -608,10 +602,10 @@
         <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8">
         <v>96251</v>
@@ -619,63 +613,42 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>7412</v>
+        <v>962</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="F10">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>54</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed additional exceptions in GUI 1
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBIT\Second Semester\EE\Project\Engineering-Exploration-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C733C2B8-BD27-40A8-9027-2CD4AC7B15B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188BC386-B417-42F7-AF81-5721F04142D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Sno</t>
   </si>
@@ -42,64 +42,61 @@
     <t>Email id</t>
   </si>
   <si>
+    <t>ASDF</t>
+  </si>
+  <si>
+    <t>qdy dfef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qrtyw </t>
+  </si>
+  <si>
+    <t>aassw</t>
+  </si>
+  <si>
+    <t>weff_</t>
+  </si>
+  <si>
+    <t>eef</t>
+  </si>
+  <si>
+    <t>deed</t>
+  </si>
+  <si>
+    <t>eefv</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>dhruv162002@gmail.com</t>
+  </si>
+  <si>
+    <t>Dhruv Saxena</t>
+  </si>
+  <si>
+    <t>TopGear</t>
+  </si>
+  <si>
+    <t>The Grand Tour</t>
+  </si>
+  <si>
+    <t>The Office,   TopGear, Sherlock</t>
+  </si>
+  <si>
+    <t>The Office, TopGear</t>
+  </si>
+  <si>
+    <t>Sherlock,  TopGear</t>
+  </si>
+  <si>
+    <t>The Office, Sherlock, TopGear, The Grand Tour</t>
+  </si>
+  <si>
     <t>Choices</t>
-  </si>
-  <si>
-    <t>ASDF</t>
-  </si>
-  <si>
-    <t>qdy dfef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qrtyw </t>
-  </si>
-  <si>
-    <t>aassw</t>
-  </si>
-  <si>
-    <t>weff_</t>
-  </si>
-  <si>
-    <t>eef</t>
-  </si>
-  <si>
-    <t>deed</t>
-  </si>
-  <si>
-    <t>eefv</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>A,   B,  C</t>
-  </si>
-  <si>
-    <t>A, B, C, D</t>
-  </si>
-  <si>
-    <t>B,  C</t>
-  </si>
-  <si>
-    <t>dhruv162002@gmail.com</t>
-  </si>
-  <si>
-    <t>Dhruv Saxena</t>
   </si>
 </sst>
 </file>
@@ -431,14 +428,14 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.77734375" customWidth="1"/>
     <col min="5" max="5" width="26.109375" customWidth="1"/>
     <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
@@ -454,13 +451,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -468,16 +465,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>74123698</v>
@@ -488,16 +485,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>852698</v>
@@ -508,16 +505,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>741</v>
@@ -528,7 +525,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>48</v>
@@ -537,7 +534,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>123698</v>
@@ -548,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>962147</v>
@@ -568,16 +565,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>412</v>
@@ -588,16 +585,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>96251</v>
@@ -608,16 +605,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <v>962</v>
@@ -628,16 +625,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F10">
         <v>8978383634</v>

</xml_diff>